<commit_message>
Updated status for 13th April
</commit_message>
<xml_diff>
--- a/Daily Status update Report 13-04-2020.xlsx
+++ b/Daily Status update Report 13-04-2020.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="149">
   <si>
     <t>Sr.No</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t xml:space="preserve">Read FD for Settlement Orchestrator and prepared Flow for the same; </t>
+  </si>
+  <si>
+    <t>Understanding Modified Trade flow; Preparation of test cases for modified trade flow</t>
   </si>
 </sst>
 </file>
@@ -7898,7 +7901,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -8165,7 +8168,9 @@
       <c r="F12" s="38">
         <v>0.75</v>
       </c>
-      <c r="G12" s="48"/>
+      <c r="G12" s="48" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="35">

</xml_diff>